<commit_message>
MongoDB -added all countries; and added method fpr geting the to sql.
Some data changes
</commit_message>
<xml_diff>
--- a/New folder/Weapons - Inventory.xlsx
+++ b/New folder/Weapons - Inventory.xlsx
@@ -1,24 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Git\Telerik Academy\Team Works\Sodium\Weapon-system-DB\New folder\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="983" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="983"/>
   </bookViews>
   <sheets>
-    <sheet name="Pistols" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Shotguns" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Submachine Guns" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Rifles" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Sniper Rifles" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Machine Guns" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Pistols" sheetId="1" r:id="rId1"/>
+    <sheet name="Shotguns" sheetId="2" r:id="rId2"/>
+    <sheet name="Submachine Guns" sheetId="3" r:id="rId3"/>
+    <sheet name="Rifles" sheetId="4" r:id="rId4"/>
+    <sheet name="Sniper Rifles" sheetId="5" r:id="rId5"/>
+    <sheet name="Machine Guns" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" name="LOCAL_MYSQL_DATE_FORMAT" vbProcedure="false">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -58,7 +62,7 @@
     <t>http://vignette1.wikia.nocookie.net/cswikia/images/c/cb/Weapon_deagle.png/revision/latest/scale-to-width-down/250?cb=20130903115839</t>
   </si>
   <si>
-    <t>Baretta 92 </t>
+    <t>Baretta 92</t>
   </si>
   <si>
     <t>Baretta</t>
@@ -151,7 +155,7 @@
     <t>Saiga-12</t>
   </si>
   <si>
-    <t>Izhmash </t>
+    <t>Izhmash</t>
   </si>
   <si>
     <t>MAC-10</t>
@@ -352,11 +356,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-  </numFmts>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -365,22 +366,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -403,7 +389,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -411,85 +397,345 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="1:11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMJ11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.5714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8061224489796"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.8622448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8520408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.72959183673469"/>
+    <col min="1" max="1" width="15.5703125"/>
+    <col min="2" max="2" width="25.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875"/>
+    <col min="4" max="4" width="18.85546875"/>
+    <col min="5" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -502,14 +748,14 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="AME1" s="0"/>
-      <c r="AMF1" s="0"/>
-      <c r="AMG1" s="0"/>
-      <c r="AMH1" s="0"/>
-      <c r="AMI1" s="0"/>
-      <c r="AMJ1" s="0"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AME1"/>
+      <c r="AMF1"/>
+      <c r="AMG1"/>
+      <c r="AMH1"/>
+      <c r="AMI1"/>
+      <c r="AMJ1"/>
+    </row>
+    <row r="2" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -523,21 +769,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="n">
+      <c r="C3" s="2">
         <v>0.5</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -551,7 +797,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -565,85 +811,85 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="2" t="n">
-        <v>0.357</v>
+      <c r="C6" s="2">
+        <v>0.35699999999999998</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="2" t="n">
-        <v>0.357</v>
+      <c r="C7" s="2">
+        <v>0.35699999999999998</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="2" t="n">
-        <v>0.357</v>
+      <c r="C8" s="2">
+        <v>0.35699999999999998</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="2" t="n">
+      <c r="C9" s="2">
         <v>0.45</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="2" t="n">
+      <c r="C10" s="2">
         <v>0.5</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="2" t="n">
-        <v>0.357</v>
+      <c r="C11" s="2">
+        <v>0.35699999999999998</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>32</v>
@@ -657,37 +903,29 @@
       <c r="K11" s="2"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="1:65536"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMJ5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.4285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0051020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.1479591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.72959183673469"/>
+    <col min="1" max="1" width="21.42578125"/>
+    <col min="2" max="2" width="13"/>
+    <col min="3" max="3" width="8.7109375"/>
+    <col min="4" max="4" width="23.140625"/>
+    <col min="5" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -700,101 +938,91 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="AME1" s="0"/>
-      <c r="AMF1" s="0"/>
-      <c r="AMG1" s="0"/>
-      <c r="AMH1" s="0"/>
-      <c r="AMI1" s="0"/>
-      <c r="AMJ1" s="0"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AME1"/>
+      <c r="AMF1"/>
+      <c r="AMG1"/>
+      <c r="AMH1"/>
+      <c r="AMI1"/>
+      <c r="AMJ1"/>
+    </row>
+    <row r="2" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" s="2">
         <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="2" t="n">
+      <c r="C3" s="2">
         <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="C4" s="2">
         <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="2" t="n">
+      <c r="C5" s="2">
         <v>12</v>
       </c>
       <c r="D5" s="2"/>
     </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="1:8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMJ8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.4285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0051020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.1479591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.72959183673469"/>
+    <col min="1" max="1" width="21.42578125"/>
+    <col min="2" max="2" width="13"/>
+    <col min="3" max="3" width="8.7109375"/>
+    <col min="4" max="4" width="23.140625"/>
+    <col min="5" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -807,21 +1035,21 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="AME1" s="0"/>
-      <c r="AMF1" s="0"/>
-      <c r="AMG1" s="0"/>
-      <c r="AMH1" s="0"/>
-      <c r="AMI1" s="0"/>
-      <c r="AMJ1" s="0"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AME1"/>
+      <c r="AMF1"/>
+      <c r="AMG1"/>
+      <c r="AMH1"/>
+      <c r="AMI1"/>
+      <c r="AMJ1"/>
+    </row>
+    <row r="2" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" s="2">
         <v>0.45</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -830,7 +1058,7 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>46</v>
       </c>
@@ -846,7 +1074,7 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>49</v>
       </c>
@@ -862,7 +1090,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>52</v>
       </c>
@@ -878,7 +1106,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>56</v>
       </c>
@@ -894,7 +1122,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>59</v>
       </c>
@@ -910,14 +1138,14 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="2" t="n">
+      <c r="C8" s="2">
         <v>0.45</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -927,37 +1155,29 @@
       <c r="F8" s="2"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="1:11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMJ11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.4285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0051020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.1479591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.72959183673469"/>
+    <col min="1" max="1" width="21.42578125"/>
+    <col min="2" max="2" width="13"/>
+    <col min="3" max="3" width="8.7109375"/>
+    <col min="4" max="4" width="23.140625"/>
+    <col min="5" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -970,14 +1190,14 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="AME1" s="0"/>
-      <c r="AMF1" s="0"/>
-      <c r="AMG1" s="0"/>
-      <c r="AMH1" s="0"/>
-      <c r="AMI1" s="0"/>
-      <c r="AMJ1" s="0"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AME1"/>
+      <c r="AMF1"/>
+      <c r="AMG1"/>
+      <c r="AMH1"/>
+      <c r="AMI1"/>
+      <c r="AMJ1"/>
+    </row>
+    <row r="2" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>65</v>
       </c>
@@ -991,7 +1211,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>68</v>
       </c>
@@ -1005,7 +1225,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>71</v>
       </c>
@@ -1019,7 +1239,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>74</v>
       </c>
@@ -1033,7 +1253,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>77</v>
       </c>
@@ -1047,7 +1267,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>79</v>
       </c>
@@ -1061,7 +1281,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>81</v>
       </c>
@@ -1075,7 +1295,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>83</v>
       </c>
@@ -1089,7 +1309,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>85</v>
       </c>
@@ -1103,7 +1323,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>88</v>
       </c>
@@ -1118,37 +1338,29 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="1:5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMJ5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.4285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0051020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.1479591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.72959183673469"/>
+    <col min="1" max="1" width="21.42578125"/>
+    <col min="2" max="2" width="13"/>
+    <col min="3" max="3" width="8.7109375"/>
+    <col min="4" max="4" width="23.140625"/>
+    <col min="5" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1161,14 +1373,14 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="AME1" s="0"/>
-      <c r="AMF1" s="0"/>
-      <c r="AMG1" s="0"/>
-      <c r="AMH1" s="0"/>
-      <c r="AMI1" s="0"/>
-      <c r="AMJ1" s="0"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AME1"/>
+      <c r="AMF1"/>
+      <c r="AMG1"/>
+      <c r="AMH1"/>
+      <c r="AMI1"/>
+      <c r="AMJ1"/>
+    </row>
+    <row r="2" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>90</v>
       </c>
@@ -1182,7 +1394,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>92</v>
       </c>
@@ -1196,7 +1408,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>95</v>
       </c>
@@ -1210,50 +1422,42 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>98</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="2" t="n">
+      <c r="C5" s="2">
         <v>0.5</v>
       </c>
       <c r="D5" s="2"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="1:4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMJ4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.4285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0051020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.1479591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.72959183673469"/>
+    <col min="1" max="1" width="21.42578125"/>
+    <col min="2" max="2" width="13"/>
+    <col min="3" max="3" width="8.7109375"/>
+    <col min="4" max="4" width="23.140625"/>
+    <col min="5" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1266,14 +1470,14 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="AME1" s="0"/>
-      <c r="AMF1" s="0"/>
-      <c r="AMG1" s="0"/>
-      <c r="AMH1" s="0"/>
-      <c r="AMI1" s="0"/>
-      <c r="AMJ1" s="0"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AME1"/>
+      <c r="AMF1"/>
+      <c r="AMG1"/>
+      <c r="AMH1"/>
+      <c r="AMI1"/>
+      <c r="AMJ1"/>
+    </row>
+    <row r="2" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>100</v>
       </c>
@@ -1283,11 +1487,11 @@
       <c r="C2" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>103</v>
       </c>
@@ -1297,11 +1501,11 @@
       <c r="C3" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>106</v>
       </c>
@@ -1311,17 +1515,12 @@
       <c r="C4" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" t="s">
         <v>107</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>